<commit_message>
modification de l'identification des partis socialiste VS conservateur + ajout de lignes de code indiquant les partis inclus + ajout de lignes de codes soustrayant les votes des non residents des residents (optionnelle, necessité à verifier) + création du fichier Figure.2 avec les étapes de l'obtention du ratio voulu.
</commit_message>
<xml_diff>
--- a/Donnees/2000 Madrid.xlsx
+++ b/Donnees/2000 Madrid.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{BF99F76E-57F0-4840-B8C7-18272868AD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C01924CF-3A66-4F5D-B0CB-94A145B04118}"/>
+    <workbookView minimized="1" xWindow="4440" yWindow="1860" windowWidth="16140" windowHeight="11820" xr2:uid="{C01924CF-3A66-4F5D-B0CB-94A145B04118}"/>
   </bookViews>
   <sheets>
     <sheet name="estadisticas - 2025-05-01T11560" sheetId="1" r:id="rId1"/>
@@ -1065,7 +1065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE53B58C-414D-4B21-80FD-AC81EC4659BC}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>